<commit_message>
changed fixed voltages to fixed values
</commit_message>
<xml_diff>
--- a/Messresultate.xlsx
+++ b/Messresultate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="28515" windowHeight="12585"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="28515" windowHeight="12585" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="4" r:id="rId1"/>
@@ -1657,7 +1657,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -2202,8 +2202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23:F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>